<commit_message>
GPLIM-1: Fix build issue
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
+++ b/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>Sample ID</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>ATRO5_RNA</t>
-  </si>
-  <si>
-    <t>abc</t>
   </si>
   <si>
     <t>Sort Column</t>
@@ -131,12 +128,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -601,13 +592,13 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="5"/>
+    <col min="3" max="3" width="10.875" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="38" customWidth="1"/>
@@ -629,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -650,7 +641,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>9</v>
@@ -737,7 +728,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -793,7 +784,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -852,7 +843,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -911,7 +902,7 @@
         <v>30</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -934,8 +925,8 @@
       <c r="J6" s="6">
         <v>4</v>
       </c>
-      <c r="K6" t="s">
-        <v>31</v>
+      <c r="K6">
+        <v>0</v>
       </c>
       <c r="L6">
         <v>1</v>

</xml_diff>

<commit_message>
GPLIM-1 - Updating test xls data file for missing column.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
+++ b/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="23320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38100" windowHeight="16180"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>Sample ID</t>
   </si>
@@ -122,13 +122,16 @@
   <si>
     <t>Material Type</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -223,12 +226,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,6 +251,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -254,13 +260,15 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -585,34 +593,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="38" customWidth="1"/>
     <col min="12" max="12" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.875" style="4"/>
+    <col min="13" max="13" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" style="4"/>
+    <col min="20" max="20" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,27 +652,30 @@
       <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="9" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="11" t="s">
+      <c r="N1" s="11"/>
+      <c r="O1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="11" t="s">
+      <c r="P1" s="11"/>
+      <c r="Q1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="10"/>
+      <c r="R1" s="11"/>
       <c r="S1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -719,8 +731,11 @@
       <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -772,11 +787,14 @@
       <c r="R3">
         <v>0.5</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -831,11 +849,14 @@
       <c r="R4">
         <v>0.5</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -890,11 +911,14 @@
       <c r="R5">
         <v>0.5</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="T5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -949,7 +973,10 @@
       <c r="R6">
         <v>0.5</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -962,8 +989,9 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
GPLIM-1: Fix some failing tests
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
+++ b/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="7480" windowWidth="38100" windowHeight="16180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Sample ID</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>RNA Extract from FFPE [P-ESH-0008]</t>
+  </si>
+  <si>
+    <t>On Risk</t>
   </si>
 </sst>
 </file>
@@ -239,7 +242,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -257,6 +260,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -611,32 +615,33 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:R1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="38" customWidth="1"/>
-    <col min="12" max="12" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" style="4"/>
-    <col min="20" max="20" width="8.83203125" style="9"/>
+    <col min="4" max="4" width="10.83203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="38" customWidth="1"/>
+    <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.83203125" style="4"/>
+    <col min="21" max="21" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,50 +652,53 @@
         <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="14"/>
+      <c r="N1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="14"/>
+      <c r="P1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="14"/>
+      <c r="R1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="13"/>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="14"/>
+      <c r="T1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -698,9 +706,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
@@ -719,38 +725,41 @@
       <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="T2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="U2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -760,30 +769,28 @@
       <c r="C3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="8">
+      <c r="I3" s="8">
         <v>41239</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="6">
+      <c r="K3" s="6">
         <v>1</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
         <v>0</v>
       </c>
@@ -791,28 +798,31 @@
         <v>0</v>
       </c>
       <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
         <v>1</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
         <v>2</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>0.5</v>
       </c>
-      <c r="S3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -822,59 +832,60 @@
       <c r="C4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="8">
+      <c r="I4" s="8">
         <v>41239</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <v>2</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
       <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>1</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
       <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <v>2</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0.5</v>
       </c>
-      <c r="S4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T4" s="3" t="s">
+      <c r="T4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -884,59 +895,60 @@
       <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="8">
+      <c r="I5" s="8">
         <v>41239</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <v>3</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>2</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
       <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
         <v>1</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
         <v>2</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>0.5</v>
       </c>
-      <c r="S5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T5" s="3" t="s">
+      <c r="T5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="U5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -946,64 +958,65 @@
       <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="8">
         <v>41239</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <v>4</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
       <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <v>1</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
       <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
         <v>1</v>
       </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
         <v>2</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>0.5</v>
       </c>
-      <c r="S6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GPLIM-1516: Verified test data and pushed the tests much farther along.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
+++ b/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26700" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>Susanna Hamilton</t>
   </si>
   <si>
-    <t>DNA3PI</t>
-  </si>
-  <si>
     <t>SM-3KBZE</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>GP85N</t>
   </si>
 </sst>
 </file>
@@ -232,7 +232,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -244,8 +244,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,6 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -276,17 +279,19 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -621,13 +626,14 @@
   </sheetPr>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="12" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="13" customWidth="1"/>
@@ -654,13 +660,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -681,26 +687,26 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="16"/>
+      <c r="O1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="16"/>
+      <c r="Q1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="16"/>
+      <c r="S1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="15"/>
-      <c r="S1" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="T1" s="15"/>
+      <c r="T1" s="16"/>
       <c r="U1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>8</v>
@@ -776,7 +782,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -784,7 +790,7 @@
         <v>17</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
@@ -796,16 +802,16 @@
         <v>41239</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="L3" s="6">
         <v>1</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -834,13 +840,13 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -848,7 +854,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
         <v>18</v>
@@ -859,17 +865,17 @@
       <c r="J4" s="8">
         <v>41239</v>
       </c>
-      <c r="K4" t="s">
-        <v>20</v>
+      <c r="K4" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="L4" s="6">
         <v>2</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -898,13 +904,13 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -912,7 +918,7 @@
         <v>17</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
@@ -923,8 +929,8 @@
       <c r="J5" s="8">
         <v>41239</v>
       </c>
-      <c r="K5" t="s">
-        <v>20</v>
+      <c r="K5" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="L5" s="6">
         <v>3</v>
@@ -933,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -962,13 +968,13 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -976,7 +982,7 @@
         <v>17</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
         <v>18</v>
@@ -987,14 +993,14 @@
       <c r="J6" s="8">
         <v>41239</v>
       </c>
-      <c r="K6" t="s">
-        <v>20</v>
+      <c r="K6" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="L6" s="6">
         <v>4</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <v>1</v>

</xml_diff>

<commit_message>
GPLIM-1516: Get all tests passing!
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
+++ b/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
@@ -232,8 +232,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -279,19 +281,21 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,8 +630,8 @@
   </sheetPr>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -811,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -826,10 +830,10 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="U3" s="9" t="s">
         <v>10</v>
@@ -875,7 +879,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -890,10 +894,10 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="U4" s="9" t="s">
         <v>10</v>
@@ -939,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -954,10 +958,10 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="U5" s="9" t="s">
         <v>10</v>
@@ -1003,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -1018,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="U6" s="9" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
GPLIM-1: Test was failing because of a price item name change
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
+++ b/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26700" windowHeight="11040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29540" windowHeight="17660"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>Strand Specific RNA-Seq (high coverage-50M paired reads) [P-RNA-0004]</t>
   </si>
   <si>
-    <t>DNA Extract from Blood, Fresh Frozen Tissue, cell pellet, stool, saliva [P-ESH-0004]</t>
-  </si>
-  <si>
     <t>RNA Extract from FFPE [P-ESH-0008]</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>GP85N</t>
+  </si>
+  <si>
+    <t>DNA or RNA Extract from Blood, Fresh Frozen Tissue, cell pellet, stool, saliva [P-ESH-0004]</t>
   </si>
 </sst>
 </file>
@@ -232,8 +232,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -281,7 +291,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -289,6 +299,11 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -296,6 +311,11 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -630,8 +650,8 @@
   </sheetPr>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -667,10 +687,10 @@
         <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -698,7 +718,7 @@
       </c>
       <c r="N1" s="16"/>
       <c r="O1" s="15" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="P1" s="16"/>
       <c r="Q1" s="17" t="s">
@@ -706,7 +726,7 @@
       </c>
       <c r="R1" s="16"/>
       <c r="S1" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T1" s="16"/>
       <c r="U1" s="1" t="s">
@@ -806,7 +826,7 @@
         <v>41239</v>
       </c>
       <c r="K3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L3" s="6">
         <v>1</v>
@@ -870,7 +890,7 @@
         <v>41239</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L4" s="6">
         <v>2</v>
@@ -934,7 +954,7 @@
         <v>41239</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L5" s="6">
         <v>3</v>
@@ -998,7 +1018,7 @@
         <v>41239</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L6" s="6">
         <v>4</v>

</xml_diff>

<commit_message>
GPLIM-512: Added lane count to PDO list and billing tracker download.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
+++ b/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="29540" windowHeight="17660"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Sample ID</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>DNA or RNA Extract from Blood, Fresh Frozen Tissue, cell pellet, stool, saliva [P-ESH-0004]</t>
+  </si>
+  <si>
+    <t>Lane Count</t>
   </si>
 </sst>
 </file>
@@ -259,7 +262,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,6 +280,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -648,35 +652,40 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:P1"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="12" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" customWidth="1"/>
-    <col min="13" max="13" width="38" customWidth="1"/>
-    <col min="14" max="14" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.83203125" style="4"/>
-    <col min="22" max="22" width="8.83203125" style="9"/>
+    <col min="6" max="6" width="46.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" customWidth="1"/>
+    <col min="14" max="14" width="38" customWidth="1"/>
+    <col min="15" max="15" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.83203125" style="4"/>
+    <col min="23" max="23" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,38 +714,41 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="17"/>
+      <c r="P1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="17" t="s">
+      <c r="Q1" s="17"/>
+      <c r="R1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="16"/>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="17"/>
+      <c r="T1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="17"/>
+      <c r="V1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -758,47 +770,48 @@
       <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="V2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="W2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -822,29 +835,29 @@
       <c r="I3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="15">
+        <v>1</v>
+      </c>
+      <c r="K3" s="8">
         <v>41239</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="6">
-        <v>1</v>
-      </c>
-      <c r="M3">
+      <c r="M3" s="6">
         <v>1</v>
       </c>
       <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>0.5</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
       <c r="P3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -855,14 +868,17 @@
       <c r="T3">
         <v>0</v>
       </c>
-      <c r="U3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="V3" s="3" t="s">
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -886,29 +902,29 @@
       <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="15">
+        <v>2</v>
+      </c>
+      <c r="K4" s="8">
         <v>41239</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="L4" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="6">
+      <c r="M4" s="6">
         <v>2</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
       <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>0.5</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
       <c r="P4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -917,16 +933,19 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="V4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -950,29 +969,29 @@
       <c r="I5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="15">
+        <v>3</v>
+      </c>
+      <c r="K5" s="8">
         <v>41239</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="L5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="6">
+      <c r="M5" s="6">
         <v>3</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
       <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
         <v>0.5</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
       <c r="P5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -981,16 +1000,19 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="V5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1014,29 +1036,26 @@
       <c r="I6" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="8">
+      <c r="K6" s="8">
         <v>41239</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="L6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="6">
+      <c r="M6" s="6">
         <v>4</v>
       </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
       <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
         <v>0.5</v>
       </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
       <c r="P6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1047,19 +1066,22 @@
       <c r="T6">
         <v>0</v>
       </c>
-      <c r="U6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="V6" s="3" t="s">
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GPLIM-1: Coaxed BillingTrackerImporterContainerTest into passing (after its product was discontinued and its primary price item changed) by hacking up the test spreadsheet and changing expectations.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
+++ b/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="3200" windowWidth="25040" windowHeight="14420"/>
+    <workbookView xWindow="2560" yWindow="720" windowWidth="31700" windowHeight="18980"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>Sample ID</t>
   </si>
@@ -160,13 +160,32 @@
   </si>
   <si>
     <t>Anopheles atroparvus EBRO</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Materials</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Billed</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -314,6 +333,22 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -378,10 +413,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -466,8 +505,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -797,22 +843,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U6" sqref="U6"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="13" width="15.1640625" customWidth="1"/>
-    <col min="14" max="25" width="25.33203125" customWidth="1"/>
-    <col min="26" max="26" width="60.6640625" customWidth="1"/>
-    <col min="27" max="27" width="101.1640625" customWidth="1"/>
+    <col min="14" max="27" width="25.33203125" customWidth="1"/>
+    <col min="28" max="28" width="60.6640625" customWidth="1"/>
+    <col min="29" max="29" width="101.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="60" customHeight="1">
+    <row r="1" spans="1:29" ht="60" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -858,44 +904,50 @@
       <c r="O1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="S1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="U1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="23" t="s">
+      <c r="V1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="24" t="s">
+      <c r="W1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="X1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="Y1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="Z1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="28" t="s">
+      <c r="AA1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -936,18 +988,18 @@
       <c r="O2">
         <v>0.5</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="2">
         <v>0</v>
       </c>
       <c r="Q2">
+        <v>0.5</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
         <v>1</v>
       </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
       <c r="T2">
         <v>0</v>
       </c>
@@ -966,11 +1018,17 @@
       <c r="Y2">
         <v>0</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1011,41 +1069,47 @@
       <c r="O3">
         <v>0.5</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="2">
         <v>0</v>
       </c>
       <c r="Q3">
+        <v>0.5</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>1</v>
       </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
       <c r="T3">
         <v>0</v>
       </c>
       <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
         <v>1</v>
       </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
       <c r="X3">
         <v>0</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1086,41 +1150,47 @@
       <c r="O4">
         <v>0.5</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="2">
         <v>0</v>
       </c>
       <c r="Q4">
+        <v>0.5</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
         <v>1</v>
       </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
       <c r="T4">
         <v>0</v>
       </c>
       <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
         <v>1</v>
       </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
       <c r="X4">
         <v>0</v>
       </c>
       <c r="Y4">
         <v>0</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1161,18 +1231,18 @@
       <c r="O5">
         <v>0.5</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="2">
         <v>0</v>
       </c>
       <c r="Q5">
+        <v>0.5</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
         <v>1</v>
       </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
       <c r="T5">
         <v>0</v>
       </c>
@@ -1191,12 +1261,19 @@
       <c r="Y5">
         <v>0</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
GPLIM-3146.  Updated price item referenced in test.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
+++ b/mercury/src/test/resources/testdata/BillingTracker-ContainerTest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="720" windowWidth="31700" windowHeight="18980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
@@ -66,10 +66,6 @@
   <si>
     <t>[P-RNA-0004]
 Update Quantity To</t>
-  </si>
-  <si>
-    <t>DNA or RNA Extract from Blood, Fresh Frozen Tissue, cell pellet, stool, saliva
-Billed</t>
   </si>
   <si>
     <t>[P-ESH-0004]
@@ -180,23 +176,22 @@
 Billed</t>
     </r>
   </si>
+  <si>
+    <t>DNA or RNA Extract from Fresh Frozen Tissue, Cell Pellet, Stool, Saliva
+Billed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -415,10 +410,10 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -477,35 +472,35 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -845,9 +840,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2:P5"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -904,80 +899,80 @@
       <c r="O1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="30" t="s">
-        <v>43</v>
+      <c r="P1" s="29" t="s">
+        <v>42</v>
       </c>
       <c r="Q1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="T1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="V1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="23" t="s">
+      <c r="W1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="X1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="Y1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="Z1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="AA1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:29">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="28">
+        <v>41239</v>
+      </c>
+      <c r="L2" t="s">
         <v>34</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="29">
-        <v>41239</v>
-      </c>
-      <c r="L2" t="s">
-        <v>35</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -1025,40 +1020,40 @@
         <v>0</v>
       </c>
       <c r="AB2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>33</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="28">
+        <v>41239</v>
+      </c>
+      <c r="L3" t="s">
         <v>34</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="29">
-        <v>41239</v>
-      </c>
-      <c r="L3" t="s">
-        <v>35</v>
       </c>
       <c r="M3">
         <v>2</v>
@@ -1106,40 +1101,40 @@
         <v>0</v>
       </c>
       <c r="AB3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
       <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>33</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="3"/>
+      <c r="K4" s="28">
+        <v>41239</v>
+      </c>
+      <c r="L4" t="s">
         <v>34</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="29">
-        <v>41239</v>
-      </c>
-      <c r="L4" t="s">
-        <v>35</v>
       </c>
       <c r="M4">
         <v>3</v>
@@ -1187,40 +1182,40 @@
         <v>0</v>
       </c>
       <c r="AB4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
       <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>32</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>33</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" s="3"/>
+      <c r="K5" s="28">
+        <v>41239</v>
+      </c>
+      <c r="L5" t="s">
         <v>34</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="29">
-        <v>41239</v>
-      </c>
-      <c r="L5" t="s">
-        <v>35</v>
       </c>
       <c r="M5">
         <v>4</v>
@@ -1268,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="AB5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>